<commit_message>
Added function to prepare networkin input for human data
</commit_message>
<xml_diff>
--- a/data/imported/phospho_human.xlsx
+++ b/data/imported/phospho_human.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="105">
   <si>
     <t xml:space="preserve">PhosphoSite</t>
   </si>
@@ -37,307 +37,307 @@
     <t xml:space="preserve">Peptides</t>
   </si>
   <si>
-    <t xml:space="preserve">CSNK1G2-Phospho:S366.S381</t>
+    <t xml:space="preserve">FAM122B-Phospho:S50.S58</t>
   </si>
   <si>
     <t xml:space="preserve">NA</t>
   </si>
   <si>
-    <t xml:space="preserve">PCDH7-Phospho:S1011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTUD4-Phospho:S1023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAT-Phospho:S40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2SURP-Phospho:S63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNX16-Phospho:S29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZNF592-Phospho:S1205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTF2F1-Phospho:S218.S221.S224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARID2-Phospho:S631.S635</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHAMP1-Phospho:S319</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NFIA-Phospho:S333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRRM2-Phospho:S1890.T1892</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUP214-Phospho:S430.S433.T437</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDC23-Phospho:S588.S593</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FNIP1-Phospho:S593.S594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEATR6-Phospho:S336.S337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUP153-Phospho:S614.S619</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZNF592-Phospho:S74.S78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRRM2-Phospho:S778.S780</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SASH3-Phospho:S357</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRS2-Phospho:S735.S736</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NKAP-Phospho:S149.S157.T161</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANKRD17-Phospho:S1696.S1700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZBTB16-Phospho:T282</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NFIA-Phospho:S258</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRSF8-Phospho:S273.S282</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA2G4-Phospho:T386</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VCPIP1-Phospho:S998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KMT2A-Phospho:S534</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPATCH8-Phospho:S911.S914</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRRM1-Phospho:S694.S696</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNMT3A-Phospho:S243.T257.T261</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HELZ-Phospho:S1738.S1741</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELL-Phospho:S444</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPTBN1-Phospho:S2319.T2320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NFATC2-Phospho:S755.S757</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EI24-Phospho:S320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MRPS17-Phospho:S127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TNIK-Phospho:S707</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NCOR2-Phospho:S2046.S2054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRRM2-Phospho:S1541.S1552</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DDX55-Phospho:S594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HUWE1-Phospho:S3906.T3924</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TARBP2-Phospho:S152</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRRM2-Phospho:S2100.S2102.T2104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHD8-Phospho:S1995.S2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLDN23-Phospho:S203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HERC2-Phospho:S1942</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DDX21-Phospho:S171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOP1-Phospho:S245.S249</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZFP36L2-Phospho:S438.S474</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WAC-Phospho:S94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELF1-Phospho:T180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SENP6-Phospho:S335.S336</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAS1L-Phospho:S249.S254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IWS1-Phospho:S261.S263</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSPA4-Phospho:S828</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZNRF2-Phospho:S116</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QSER1-Phospho:T1341.S1348</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPO-Phospho:S92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLEKHO2-Phospho:S273</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRKCA-Phospho:T638.S657</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EFHD2-Phospho:S76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNMT3B-Phospho:S82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSF1-Phospho:S617.T628</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RREB1-Phospho:S1167.S1174</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HNRNPD-Phospho:S82.S83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAM114A2-Phospho:S146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAM122A-Phospho:S270</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MINK1-Phospho:S732</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHD4-Phospho:S515</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUD13-Phospho:S172.S175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNAPC4-Phospho:S1224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAPGEF6-Phospho:S1229.S1241</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHKBP1-Phospho:S642.S649</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPAP3-Phospho:S116.S119.S121</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRF2-Phospho:S144</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARID4B-Phospho:S1029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CASC3-Phospho:T127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAV1-Phospho:S452</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEX10-Phospho:S261</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TBC1D9B-Phospho:T1239</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CENPC-Phospho:S73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATXN2-Phospho:T529</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PNMA5-Phospho:S128.S133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UBAP2L-Phospho:S605.S609</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHD7-Phospho:S2559</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABI1-Phospho:S183.T191</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARCKSL1-Phospho:S162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZNF687-Phospho:T1120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEBPZ-Phospho:S34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KIF1B-Phospho:S1057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCM1-Phospho:S378.S380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TPR-Phospho:S646</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WWOX-Phospho:T12.S14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSPH1-Phospho:S809.T815</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRPF40A-Phospho:S933.S935.S938</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCRIB-Phospho:S1306.S1309</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDS2-Phospho:S33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATXN7L3-Phospho:S131</t>
+    <t xml:space="preserve">IRF8-Phospho:S162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RANBP3-Phospho:S241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PNCK-Phospho:S283.S285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAPK1-Phospho:T185.Y187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAP3K11-Phospho:S548</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SH2B3-Phospho:S141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVPL-Phospho:S1617.T1624.S1626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SH3RF3-Phospho:S797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VPS13B-Phospho:S1815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPP1R1B-Phospho:S45.S46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPL3-Phospho:S13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NYAP2-Phospho:T220.S221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LRRFIP1-Phospho:S713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCHS1-Phospho:S827.S829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTA2-Phospho:S548</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDK12-Phospho:S332.S334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARHGAP45-Phospho:S577.S578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YBX1-Phospho:S165.S176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BDP1-Phospho:S1317</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIGYF2-Phospho:S236.S242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SF3B1-Phospho:T244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STIM1-Phospho:S512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP6V1C2-Phospho:S54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPS6KA4-Phospho:S343.S347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIN2-Phospho:T276.S277</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIST1H1B-Phospho:S189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KLB-Phospho:S799.S800.S801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDI2-Phospho:S121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEFV-Phospho:S179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPEF2-Phospho:S353.S356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZNF654-Phospho:S576.S580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCSK7-Phospho:S502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HNRNPUL2-Phospho:S193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRRC2A-Phospho:S920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPAN-Phospho:S238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THRAP3-Phospho:S408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCF12-Phospho:S116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLR1D-Phospho:S100.S104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPATCH8-Phospho:S1009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCL6-Phospho:S333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRS2-Phospho:S1148.S1149.S1162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1FX-Phospho:S27.S33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRRM2-Phospho:S1916.S1919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MON1B-Phospho:S59.S61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KDM2B-Phospho:S1029.S1031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNF25-Phospho:S450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZC3H13-Phospho:S207.S211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZC3H13-Phospho:S370.S372.S380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACIN1-Phospho:S388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPAP3-Phospho:S245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSUN5P2-Phospho:S260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDK14-Phospho:S78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRIP12-Phospho:S310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUNX3-Phospho:S227.T231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BZW1-Phospho:S411.S413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCOR1-Phospho:S70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRRM2-Phospho:S1890.S1893</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PNKP-Phospho:S114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPRD1B-Phospho:S132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNPS1-Phospho:S137.S139.S141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUP133-Phospho:S57.T63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZNF318-Phospho:S89.S91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCNE2-Phospho:S21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SON-Phospho:S2020.T2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTF3C1-Phospho:S1854</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYO9B-Phospho:S1356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DENND1C-Phospho:S582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHACTR4-Phospho:S270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENPA-Phospho:S17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POM121-Phospho:S179.S188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTPN22-Phospho:S493</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRPF38B-Phospho:S266.S268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCL7C-Phospho:T111.S126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRKACB-Phospho:S339</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYOCD-Phospho:S577.S578.S583</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LRWD1-Phospho:S212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALAS1-Phospho:S85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARHGAP22-Phospho:S587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIT1-Phospho:S385.S388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIDO1-Phospho:T1256.S1260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EAF2-Phospho:S144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRRM1-Phospho:S450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MADD-Phospho:S813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRRM2-Phospho:S1972.S1975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIST1H1B-Phospho:T138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AHNAK-Phospho:S4986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYO9B-Phospho:S1405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBN2-Phospho:S584</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EIF4B-Phospho:S442.S445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATXN2L-Phospho:T683</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DVL2-Phospho:S169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFT2D1-Phospho:S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIN37-Phospho:S182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDK14-Phospho:S134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARK3-Phospho:S563.T564</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TBC1D9B-Phospho:S411.S435</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTMR1-Phospho:S653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHRF1-Phospho:S936.S950.T951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IWS1-Phospho:S511.S513</t>
   </si>
 </sst>
 </file>
@@ -445,8 +445,8 @@
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -494,7 +494,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,13 +516,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>5</v>
+        <v>-5.21868254383863</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.0763412259565217</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -530,13 +530,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>-1000</v>
+        <v>-4.87891443404146</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,13 +544,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>5</v>
+        <v>-4.7589370954364</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.00238506146040802</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -558,13 +558,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>5</v>
+        <v>-4.58341910734125</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.0252662801278472</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,13 +572,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>5</v>
+        <v>-4.25585565221996</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.0581756240455477</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,13 +586,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>-1000</v>
+        <v>-4.02023043503224</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -600,13 +600,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>-1000</v>
+        <v>-3.92258885831679</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,13 +614,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>5</v>
+        <v>-3.69324733448973</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.306736705868602</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,13 +628,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>-1000</v>
+        <v>-3.65975915544892</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,13 +642,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>5</v>
+        <v>-3.65285057707532</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.499225885890268</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,13 +656,13 @@
         <v>18</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>5</v>
+        <v>-3.43804562815701</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.29457120738987</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,13 +670,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>5</v>
+        <v>-3.43308784693499</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.43173774368499</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -684,13 +684,13 @@
         <v>20</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>5</v>
+        <v>-3.39159134342557</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.550659082446883</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -698,13 +698,13 @@
         <v>21</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>-1000</v>
+        <v>-3.31844798378315</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,13 +712,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>-1000</v>
+        <v>-3.29844697754506</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,13 +726,13 @@
         <v>23</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>-1000</v>
+        <v>-3.29274922350289</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,13 +740,13 @@
         <v>24</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>5</v>
+        <v>-3.26286859941313</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.013182461429139</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,13 +754,13 @@
         <v>25</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>5</v>
+        <v>-3.23413171802306</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0.0282072072430804</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,13 +768,13 @@
         <v>26</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>-1000</v>
+        <v>-3.1609999038515</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,13 +782,13 @@
         <v>27</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>-1000</v>
+        <v>-3.13827162930331</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,13 +796,13 @@
         <v>28</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>-1000</v>
+        <v>-3.10239257716916</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,13 +810,13 @@
         <v>29</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>5</v>
+        <v>-3.09924573239681</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0.375828412063727</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,13 +824,13 @@
         <v>30</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>-1000</v>
+        <v>-3.08074102435223</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,13 +838,13 @@
         <v>31</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>5</v>
+        <v>-3.0259784540963</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0.460508294541169</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,13 +852,13 @@
         <v>32</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>-1000</v>
+        <v>-3.01885766276732</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,13 +866,13 @@
         <v>33</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>5</v>
+        <v>-2.90093695980286</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0.611594205112674</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,13 +880,13 @@
         <v>34</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>5</v>
+        <v>-2.83643510731873</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0.193365751819354</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,13 +894,13 @@
         <v>35</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>5</v>
+        <v>-2.80481218789807</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0.201652875646623</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,13 +908,13 @@
         <v>36</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.75316618131815</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,13 +922,13 @@
         <v>37</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>5</v>
+        <v>-2.7357803717279</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0.0441214695478543</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,13 +936,13 @@
         <v>38</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.67025591132703</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,13 +950,13 @@
         <v>39</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>5</v>
+        <v>-2.65222279357336</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>0.359040367584651</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,13 +964,13 @@
         <v>40</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.61869635791355</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,13 +978,13 @@
         <v>41</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.6169936746986</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,13 +992,13 @@
         <v>42</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>5</v>
+        <v>-2.58337255026201</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>0.123993786409964</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,13 +1006,13 @@
         <v>43</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>5</v>
+        <v>-2.47169381127091</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>0.72402883385193</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1020,13 +1020,13 @@
         <v>44</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.45111984581126</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1034,13 +1034,13 @@
         <v>45</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.38171142677332</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,13 +1048,13 @@
         <v>46</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>5</v>
+        <v>-2.31875341189096</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>0.406232344260693</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,13 +1062,13 @@
         <v>47</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>5</v>
+        <v>-2.30633174125993</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>0.329298829047284</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,13 +1076,13 @@
         <v>48</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.28713955524258</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,7 +1090,7 @@
         <v>49</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.27936956162404</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>5</v>
@@ -1104,13 +1104,13 @@
         <v>50</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>5</v>
+        <v>-2.27802333972589</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>0.435844514205287</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,13 +1118,13 @@
         <v>51</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.24514146629764</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,13 +1132,13 @@
         <v>52</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>5</v>
+        <v>-2.22954459189336</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>0.421442621301397</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,13 +1146,13 @@
         <v>53</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>5</v>
+        <v>-2.22398253485687</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>0.603116026380029</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,13 +1160,13 @@
         <v>54</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>5</v>
+        <v>-2.21963530939549</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>0.110945102644545</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,13 +1174,13 @@
         <v>55</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>5</v>
+        <v>-2.21854335225825</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>0.0256918869330322</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,13 +1188,13 @@
         <v>56</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.21729573221236</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,13 +1202,13 @@
         <v>57</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>5</v>
+        <v>-2.21170700592118</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>0.0473154266723747</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1216,13 +1216,13 @@
         <v>58</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>5</v>
+        <v>-2.21035718833618</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>0.143820149476276</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,13 +1230,13 @@
         <v>59</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.21004591720107</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,13 +1244,13 @@
         <v>60</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.19626801425575</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1258,13 +1258,13 @@
         <v>61</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.13946860941729</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,13 +1272,13 @@
         <v>62</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>5</v>
+        <v>-2.12643839573698</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>0.579845431128839</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,13 +1286,13 @@
         <v>63</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.12601758010882</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,13 +1300,13 @@
         <v>64</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.12360706883009</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,13 +1314,13 @@
         <v>65</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.11392730215514</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,13 +1328,13 @@
         <v>66</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.1045890709155</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,13 +1342,13 @@
         <v>67</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>5</v>
+        <v>-2.09999188484241</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>0.668762328540604</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,13 +1356,13 @@
         <v>68</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>5</v>
+        <v>-2.09312962280605</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>0.806423589041931</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,13 +1370,13 @@
         <v>69</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>5</v>
+        <v>-2.09225273107658</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>0.659898106458811</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,13 +1384,13 @@
         <v>70</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.0716066116072</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,13 +1398,13 @@
         <v>71</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>5</v>
+        <v>-2.07006578439247</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>0.0126061555277647</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1412,13 +1412,13 @@
         <v>72</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>5</v>
+        <v>-2.05449957432503</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>0.181735460696714</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1426,13 +1426,13 @@
         <v>73</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.0533455381485</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,13 +1440,13 @@
         <v>74</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>5</v>
+        <v>-2.04192828160994</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>0.506951246106053</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,13 +1454,13 @@
         <v>75</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>5</v>
+        <v>-2.01923591091136</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>0.0682666638638291</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,13 +1468,13 @@
         <v>76</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>5</v>
+        <v>-2.00342874907986</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>0.170525533033788</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,13 +1482,13 @@
         <v>77</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>5</v>
+        <v>-2.00256737400228</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>0.514548048207413</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,13 +1496,13 @@
         <v>78</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>-1000</v>
+        <v>-2.00189505288249</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,13 +1510,13 @@
         <v>79</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.98854697299936</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,13 +1524,13 @@
         <v>80</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.98745923662479</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,13 +1538,13 @@
         <v>81</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.98462715123197</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,13 +1552,13 @@
         <v>82</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.97601747245655</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,13 +1566,13 @@
         <v>83</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>5</v>
+        <v>-1.94805830576893</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>0.66908351156676</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,13 +1580,13 @@
         <v>84</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.94424436741812</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,13 +1594,13 @@
         <v>85</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>5</v>
+        <v>-1.92827323996492</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>0.51925031213179</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,13 +1608,13 @@
         <v>86</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>5</v>
+        <v>-1.92155814801878</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>0.725424393211702</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,13 +1622,13 @@
         <v>87</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>5</v>
+        <v>-1.92006512462839</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>0.188684640729358</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1636,13 +1636,13 @@
         <v>88</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.91883511063696</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,13 +1650,13 @@
         <v>89</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>5</v>
+        <v>-1.91698206373353</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>0.569289024912328</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,13 +1664,13 @@
         <v>90</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.91425645886021</v>
       </c>
       <c r="C87" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,13 +1678,13 @@
         <v>91</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>5</v>
+        <v>-1.91128646635137</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>0.149080295282231</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,13 +1692,13 @@
         <v>92</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>5</v>
+        <v>-1.91073259220095</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>0.287302616947581</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,13 +1706,13 @@
         <v>93</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.90830122190369</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,13 +1720,13 @@
         <v>94</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>5</v>
+        <v>-1.90562690112447</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>0.35135608435763</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,13 +1734,13 @@
         <v>95</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.90196202372564</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,13 +1748,13 @@
         <v>96</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.89407349006983</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,13 +1762,13 @@
         <v>97</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>5</v>
+        <v>-1.87009437500949</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>0.267935365571585</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,13 +1776,13 @@
         <v>98</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.86562687759813</v>
       </c>
       <c r="C95" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,13 +1790,13 @@
         <v>99</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C96" s="0" t="s">
-        <v>5</v>
+        <v>-1.86184152416101</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>0.103755718077858</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,13 +1804,13 @@
         <v>100</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C97" s="0" t="s">
-        <v>5</v>
+        <v>-1.86056504808748</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>0.212050560176861</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,13 +1818,13 @@
         <v>101</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>5</v>
+        <v>-1.86050395439476</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>0.167167553232508</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1832,13 +1832,13 @@
         <v>102</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.85373680397719</v>
       </c>
       <c r="C99" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,13 +1846,13 @@
         <v>103</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>-1000</v>
+        <v>-1.83779313407275</v>
       </c>
       <c r="C100" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,13 +1860,13 @@
         <v>104</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>5</v>
+        <v>-1.83188575538244</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>0.550659082446883</v>
       </c>
       <c r="D101" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>